<commit_message>
added additional data tables...
</commit_message>
<xml_diff>
--- a/data/Inversions_data_snps_SVs_genes.xlsx
+++ b/data/Inversions_data_snps_SVs_genes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesliekollar/Desktop/Mimulus_genome_assembly/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D619FE13-6F70-D84B-8288-DE52128632A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186CA629-AAFB-FF4D-AE4A-13BF5A65CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30020" yWindow="-2440" windowWidth="27640" windowHeight="16440" xr2:uid="{0B782887-C230-A94B-AA47-4B8299107935}"/>
+    <workbookView xWindow="-38160" yWindow="-3100" windowWidth="24900" windowHeight="16440" xr2:uid="{0B782887-C230-A94B-AA47-4B8299107935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>LMC SNPs</t>
   </si>
@@ -50,12 +50,6 @@
     <t>SWB size</t>
   </si>
   <si>
-    <t>LMC Genes with SNPS</t>
-  </si>
-  <si>
-    <t>SWB Genes with SNPS</t>
-  </si>
-  <si>
     <t>4,196,511 bp</t>
   </si>
   <si>
@@ -86,15 +80,6 @@
     <t>2,784,925 bp</t>
   </si>
   <si>
-    <t>LMC specific gene content</t>
-  </si>
-  <si>
-    <t>SWB specific gene content</t>
-  </si>
-  <si>
-    <t>Shared gene content</t>
-  </si>
-  <si>
     <t>Genome</t>
   </si>
   <si>
@@ -111,6 +96,9 @@
   </si>
   <si>
     <t>Chromosome 8 inversion (large inversion without small inversion)</t>
+  </si>
+  <si>
+    <t>Chromosome inversion 14</t>
   </si>
 </sst>
 </file>
@@ -500,7 +488,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1048576"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +505,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -531,51 +519,39 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3">
+        <v>6192716</v>
+      </c>
+      <c r="E2" s="3">
+        <v>6234953</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="3">
-        <v>4769</v>
-      </c>
-      <c r="I2" s="3">
-        <v>4117</v>
-      </c>
-      <c r="J2" s="3">
-        <v>18245</v>
-      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>141267</v>
@@ -585,25 +561,17 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3">
-        <v>347</v>
-      </c>
-      <c r="I3">
-        <v>281</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1090</v>
-      </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <v>8606</v>
@@ -614,13 +582,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3">
         <v>223542</v>
@@ -628,25 +596,17 @@
       <c r="E5" s="3">
         <v>181793</v>
       </c>
-      <c r="H5">
-        <v>505</v>
-      </c>
-      <c r="I5">
-        <v>423</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1915</v>
-      </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6">
         <v>214936</v>
@@ -656,14 +616,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>14</v>
+      <c r="A7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>63711</v>
@@ -671,15 +631,7 @@
       <c r="E7" s="3">
         <v>79338</v>
       </c>
-      <c r="H7">
-        <v>247</v>
-      </c>
-      <c r="I7">
-        <v>308</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1133</v>
-      </c>
+      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>